<commit_message>
1. keyword 2. sort field
</commit_message>
<xml_diff>
--- a/report_template/buildCase.xlsx
+++ b/report_template/buildCase.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -67,7 +67,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -148,10 +148,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -476,12 +476,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="6" width="14" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.25" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.75" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.125" style="2" customWidth="1"/>
     <col min="8" max="8" width="8.875" style="2"/>
-    <col min="9" max="9" width="31.875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="54.625" style="2" customWidth="1"/>
     <col min="10" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>

</xml_diff>